<commit_message>
feat(doc): remover os erros da parte de mapa de unidades
</commit_message>
<xml_diff>
--- a/documentacao/teste_maisconsulta.xlsx
+++ b/documentacao/teste_maisconsulta.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thais\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\--consulta\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862B6383-C88E-49F2-9838-BCFF41CF4168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9ECBCF-74F5-4933-868C-2F40D1D64885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F13FDC1B-4AD5-47E7-AA19-1D28F11FE616}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="106">
   <si>
     <t>Testes do sistema</t>
   </si>
@@ -202,18 +202,6 @@
   </si>
   <si>
     <t>Adicionar modal de confirmação geral de agendamento</t>
-  </si>
-  <si>
-    <t>Tela de mapa de unidades (Paciente)</t>
-  </si>
-  <si>
-    <t>Requisiçao para encontrar unidades próximas a você está errada (Está buscando por especialidade)</t>
-  </si>
-  <si>
-    <t>Ao selecionar ubs está quebrando a tela inteira</t>
-  </si>
-  <si>
-    <t>Mapa está estático</t>
   </si>
   <si>
     <t>Tela de profile</t>
@@ -718,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67F6240-8D79-49A4-8FA5-5E1579F8B412}">
-  <dimension ref="A1:D110"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="D52" sqref="D51:D52"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,10 +725,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -751,7 +739,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -759,7 +747,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -767,7 +755,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -775,7 +763,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -783,7 +771,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -791,7 +779,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -799,7 +787,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -810,7 +798,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -818,7 +806,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -826,7 +814,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -834,7 +822,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -842,7 +830,7 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -850,7 +838,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -858,7 +846,7 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -866,7 +854,7 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -874,7 +862,7 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -882,7 +870,7 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -890,7 +878,7 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -898,7 +886,7 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -906,7 +894,7 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -914,7 +902,7 @@
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -925,7 +913,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -933,7 +921,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -941,7 +929,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -952,7 +940,7 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -960,7 +948,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -968,7 +956,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -976,7 +964,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -984,7 +972,7 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -992,7 +980,7 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1000,7 +988,7 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1008,7 +996,7 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1016,7 +1004,7 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1024,7 +1012,7 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1032,7 +1020,7 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1040,7 +1028,7 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1048,7 +1036,7 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1056,7 +1044,7 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1067,7 +1055,7 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1075,7 +1063,7 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1083,7 +1071,7 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1091,7 +1079,7 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1099,7 +1087,7 @@
         <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1107,7 +1095,7 @@
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1115,7 +1103,7 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1123,10 +1111,10 @@
         <v>49</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1134,10 +1122,10 @@
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1145,7 +1133,7 @@
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1153,7 +1141,7 @@
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1161,7 +1149,7 @@
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1169,7 +1157,7 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1177,401 +1165,374 @@
         <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>56</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>57</v>
       </c>
-      <c r="C59" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>58</v>
-      </c>
       <c r="C60" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>59</v>
       </c>
-      <c r="C61" t="s">
-        <v>105</v>
+      <c r="C62" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="B63" t="s">
         <v>60</v>
       </c>
-      <c r="B63" t="s">
-        <v>61</v>
-      </c>
       <c r="C63" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C64" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C65" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C66" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C67" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C69" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C70" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C71" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C72" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>71</v>
       </c>
-      <c r="C73" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>72</v>
       </c>
-      <c r="C74" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>73</v>
-      </c>
       <c r="C75" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>105</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>75</v>
-      </c>
       <c r="B78" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="C78" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="C79" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="C80" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>24</v>
-      </c>
-      <c r="C81" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>74</v>
+      </c>
       <c r="B82" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="C82" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C83" t="s">
-        <v>106</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>77</v>
+      </c>
+      <c r="C84" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="B85" t="s">
         <v>78</v>
       </c>
-      <c r="B85" t="s">
-        <v>79</v>
-      </c>
       <c r="C85" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C86" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C87" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C88" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
+        <v>97</v>
+      </c>
+      <c r="C89" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>82</v>
+      </c>
+      <c r="B91" t="s">
         <v>83</v>
       </c>
-      <c r="C89" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>84</v>
-      </c>
-      <c r="C90" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>85</v>
-      </c>
       <c r="C91" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C92" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>85</v>
+      </c>
+      <c r="C93" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="B94" t="s">
         <v>86</v>
       </c>
-      <c r="B94" t="s">
-        <v>87</v>
-      </c>
       <c r="C94" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C95" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C96" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C97" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C98" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="C99" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C100" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C101" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C102" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>94</v>
-      </c>
-      <c r="C103" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>87</v>
+      </c>
       <c r="B104" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C104" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C105" t="s">
-        <v>105</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>70</v>
+      </c>
+      <c r="C106" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>91</v>
-      </c>
       <c r="B107" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C107" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>93</v>
-      </c>
-      <c r="C108" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>74</v>
-      </c>
-      <c r="C109" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>94</v>
-      </c>
-      <c r="C110" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(doc): mais um feito
</commit_message>
<xml_diff>
--- a/documentacao/teste_maisconsulta.xlsx
+++ b/documentacao/teste_maisconsulta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\--consulta\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9ECBCF-74F5-4933-868C-2F40D1D64885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC050BA9-9C43-4A5A-A88A-33EF5C42B0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F13FDC1B-4AD5-47E7-AA19-1D28F11FE616}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="106">
   <si>
     <t>Testes do sistema</t>
   </si>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67F6240-8D79-49A4-8FA5-5E1579F8B412}">
   <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,6 +1178,9 @@
       <c r="C60" t="s">
         <v>102</v>
       </c>
+      <c r="D60" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">

</xml_diff>

<commit_message>
feat(doc): mais alterações realizadas
</commit_message>
<xml_diff>
--- a/documentacao/teste_maisconsulta.xlsx
+++ b/documentacao/teste_maisconsulta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\--consulta\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC050BA9-9C43-4A5A-A88A-33EF5C42B0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728BEA82-DADB-4179-9975-0F8DFF0B3283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F13FDC1B-4AD5-47E7-AA19-1D28F11FE616}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="106">
   <si>
     <t>Testes do sistema</t>
   </si>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67F6240-8D79-49A4-8FA5-5E1579F8B412}">
   <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="B53" workbookViewId="0">
+      <selection activeCell="D61" sqref="D60:D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,6 +1189,9 @@
       <c r="C61" t="s">
         <v>101</v>
       </c>
+      <c r="D61" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">

</xml_diff>

<commit_message>
feat(doc): atualizar status dos processos
</commit_message>
<xml_diff>
--- a/documentacao/teste_maisconsulta.xlsx
+++ b/documentacao/teste_maisconsulta.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\--consulta\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Thais\3ADSB\--consulta\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728BEA82-DADB-4179-9975-0F8DFF0B3283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2284340D-0B42-4D5F-B37E-321C630FE5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F13FDC1B-4AD5-47E7-AA19-1D28F11FE616}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{F13FDC1B-4AD5-47E7-AA19-1D28F11FE616}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="104">
   <si>
     <t>Testes do sistema</t>
   </si>
@@ -223,12 +223,6 @@
   </si>
   <si>
     <t>Poderiam ser sinalizados os campos obrigatórios</t>
-  </si>
-  <si>
-    <t>Esticar linha ao lado do formulário</t>
-  </si>
-  <si>
-    <t>Poderia fixar a imagem ao lado quando dado o scroll</t>
   </si>
   <si>
     <t>Remover outline nos inputs</t>
@@ -706,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67F6240-8D79-49A4-8FA5-5E1579F8B412}">
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B53" workbookViewId="0">
-      <selection activeCell="D61" sqref="D60:D61"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,10 +719,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -739,7 +733,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -747,7 +741,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -755,7 +749,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -763,7 +757,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,7 +765,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -779,7 +773,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -787,7 +781,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -798,7 +792,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -806,7 +800,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -814,7 +808,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -822,7 +816,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -830,7 +824,7 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -838,7 +832,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -846,7 +840,7 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -854,7 +848,7 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -862,7 +856,7 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -870,7 +864,7 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -878,7 +872,7 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -886,7 +880,7 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -894,7 +888,7 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -902,7 +896,7 @@
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -913,7 +907,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -921,7 +915,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -929,7 +923,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -940,7 +934,7 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -948,7 +942,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -956,7 +950,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -964,90 +958,90 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -1055,39 +1049,54 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1095,7 +1104,10 @@
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1103,7 +1115,10 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1111,10 +1126,10 @@
         <v>49</v>
       </c>
       <c r="C51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1122,10 +1137,10 @@
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1133,7 +1148,10 @@
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1141,7 +1159,7 @@
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1149,7 +1167,7 @@
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1157,7 +1175,10 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1165,7 +1186,7 @@
         <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1176,10 +1197,10 @@
         <v>57</v>
       </c>
       <c r="C60" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1187,10 +1208,10 @@
         <v>58</v>
       </c>
       <c r="C61" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1198,7 +1219,7 @@
         <v>59</v>
       </c>
       <c r="C62" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1206,7 +1227,7 @@
         <v>60</v>
       </c>
       <c r="C63" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1214,141 +1235,151 @@
         <v>61</v>
       </c>
       <c r="C64" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>62</v>
       </c>
       <c r="C65" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="D65" s="1"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>63</v>
       </c>
       <c r="C66" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>64</v>
       </c>
       <c r="C67" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>66</v>
       </c>
       <c r="C69" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>67</v>
       </c>
       <c r="C70" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>68</v>
       </c>
       <c r="C71" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>69</v>
       </c>
-      <c r="C72" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>70</v>
       </c>
       <c r="C73" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>71</v>
       </c>
+      <c r="C74" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
+        <v>23</v>
+      </c>
+      <c r="C75" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>24</v>
+      </c>
+      <c r="C76" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>96</v>
+      </c>
+      <c r="C78" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>72</v>
       </c>
-      <c r="C75" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+      <c r="B80" t="s">
         <v>73</v>
       </c>
-      <c r="C76" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>23</v>
-      </c>
-      <c r="C77" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>24</v>
-      </c>
-      <c r="C78" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>25</v>
-      </c>
-      <c r="C79" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>98</v>
-      </c>
       <c r="C80" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>74</v>
+      </c>
+      <c r="C81" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>74</v>
-      </c>
       <c r="B82" t="s">
         <v>75</v>
       </c>
       <c r="C82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1356,7 +1387,7 @@
         <v>76</v>
       </c>
       <c r="C83" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1364,7 +1395,7 @@
         <v>77</v>
       </c>
       <c r="C84" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1372,7 +1403,7 @@
         <v>78</v>
       </c>
       <c r="C85" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1380,42 +1411,42 @@
         <v>79</v>
       </c>
       <c r="C86" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
+        <v>95</v>
+      </c>
+      <c r="C87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>80</v>
       </c>
-      <c r="C87" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+      <c r="B89" t="s">
         <v>81</v>
       </c>
-      <c r="C88" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>97</v>
-      </c>
       <c r="C89" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>82</v>
+      </c>
+      <c r="C90" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>82</v>
-      </c>
       <c r="B91" t="s">
         <v>83</v>
       </c>
       <c r="C91" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1423,12 +1454,12 @@
         <v>84</v>
       </c>
       <c r="C92" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C93" t="s">
         <v>100</v>
@@ -1436,10 +1467,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C94" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1447,7 +1478,7 @@
         <v>91</v>
       </c>
       <c r="C95" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1455,90 +1486,74 @@
         <v>92</v>
       </c>
       <c r="C96" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="C97" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C98" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="C99" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C100" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>95</v>
-      </c>
-      <c r="C101" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>85</v>
+      </c>
       <c r="B102" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C102" t="s">
-        <v>101</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>87</v>
+      </c>
+      <c r="C103" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>87</v>
-      </c>
       <c r="B104" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C105" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
-        <v>70</v>
-      </c>
-      <c r="C106" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>90</v>
-      </c>
-      <c r="C107" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(doc): adicionar mais feitos dentro da documentação
</commit_message>
<xml_diff>
--- a/documentacao/teste_maisconsulta.xlsx
+++ b/documentacao/teste_maisconsulta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\--consulta\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AE07D8-291F-4F7D-8EC9-002B8497A757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2801B7D-FB16-4D72-B673-209431A8BFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F13FDC1B-4AD5-47E7-AA19-1D28F11FE616}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="85">
   <si>
     <t>Testes do sistema</t>
   </si>
@@ -117,42 +117,12 @@
     <t>Tela de histórico (Paciente)</t>
   </si>
   <si>
-    <t>Tamanho incorreto entre os selects</t>
-  </si>
-  <si>
-    <t>Botões estão ficando muito distantes quando a tela é maior</t>
-  </si>
-  <si>
-    <t>Espaçamento da label com o select está muito grudado</t>
-  </si>
-  <si>
-    <t>Cinza no fundo do botão de "Baixar selecionados" está estranho</t>
-  </si>
-  <si>
-    <t>Letras muito pequenas dentro dos selects</t>
-  </si>
-  <si>
     <t>Data de consulta está com padrão de data americano (mês/dia/ano)</t>
   </si>
   <si>
-    <t>Filtro não está funcionando</t>
-  </si>
-  <si>
-    <t>Posto de saude preenchendo com campo vazio</t>
-  </si>
-  <si>
     <t>Id do paciente que está sendo enviado ao endpoint está mocado (Deveria pegar do local storage) (Estão sendo enviados aos endpoints de ubs e de historico)</t>
   </si>
   <si>
-    <t>Baixar tudo/Baixar selecionados não estão funcionando</t>
-  </si>
-  <si>
-    <t>Botão de download individual não é clicavel</t>
-  </si>
-  <si>
-    <t>Botão de download individual não está funcionando</t>
-  </si>
-  <si>
     <t>Cor do ícone de agendamento é mais claro que dos outros ícones do menu</t>
   </si>
   <si>
@@ -228,9 +198,6 @@
     <t>Não possui botão salvar nem cancelar</t>
   </si>
   <si>
-    <t>Visibilidade de quando está livre ou bloqueado os inputs poderia ser melhor</t>
-  </si>
-  <si>
     <t>Select está com alinhamento e estilização diferente dos demais</t>
   </si>
   <si>
@@ -252,21 +219,9 @@
     <t>Alinhamento não está padronizado</t>
   </si>
   <si>
-    <t>Input de busca está gigante</t>
-  </si>
-  <si>
     <t>Tamanhos estão desproporcionais</t>
   </si>
   <si>
-    <t>Lupa está descentralizado dentro do input</t>
-  </si>
-  <si>
-    <t>Busca não está clicável</t>
-  </si>
-  <si>
-    <t>Busca não está funcionando</t>
-  </si>
-  <si>
     <t>Pacientes estão mocados</t>
   </si>
   <si>
@@ -279,9 +234,6 @@
     <t>"Paciente" poderia ser o nome do paciente</t>
   </si>
   <si>
-    <t>Último atendimento caso não possua um ultimo atendimento poderia deixar uma mensagem padrão (Você não possui ultimos atendimentos)</t>
-  </si>
-  <si>
     <t>Dados estão mocados</t>
   </si>
   <si>
@@ -294,9 +246,6 @@
     <t>Remover outline dos inputs</t>
   </si>
   <si>
-    <t>Tratar erros</t>
-  </si>
-  <si>
     <t>Remover campo de atestado</t>
   </si>
   <si>
@@ -315,9 +264,6 @@
     <t>Botão de cancelar não está funcionando</t>
   </si>
   <si>
-    <t xml:space="preserve">Quando clicado em um paciente deveria abrir  tela de atendimento com todos os campos do ultimo atendimento bloqueados </t>
-  </si>
-  <si>
     <t xml:space="preserve">Icone de pacientes poderia ser diferente </t>
   </si>
   <si>
@@ -340,6 +286,9 @@
   </si>
   <si>
     <t>Feito</t>
+  </si>
+  <si>
+    <t>Baixar tudo não estão funcionando</t>
   </si>
 </sst>
 </file>
@@ -389,11 +338,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -712,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67F6240-8D79-49A4-8FA5-5E1579F8B412}">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,10 +677,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" t="s">
-        <v>100</v>
+        <v>77</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -745,56 +691,66 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -804,114 +760,131 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -919,650 +892,589 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>27</v>
       </c>
-      <c r="C29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>28</v>
       </c>
-      <c r="C30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>29</v>
-      </c>
       <c r="C31" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
+        <v>79</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" t="s">
         <v>32</v>
       </c>
-      <c r="C34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
       <c r="C36" t="s">
-        <v>97</v>
+        <v>79</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>97</v>
+        <v>79</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>79</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>79</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
+        <v>79</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>96</v>
+        <v>79</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>40</v>
       </c>
-      <c r="C42" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B44" t="s">
-        <v>42</v>
-      </c>
       <c r="C44" t="s">
-        <v>97</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>101</v>
+        <v>78</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>97</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>101</v>
+        <v>79</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>97</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>101</v>
+        <v>79</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s">
         <v>45</v>
       </c>
-      <c r="C47" t="s">
-        <v>97</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>46</v>
-      </c>
-      <c r="C48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" t="s">
-        <v>97</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>48</v>
-      </c>
       <c r="C50" t="s">
-        <v>97</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>101</v>
+        <v>80</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>96</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>101</v>
+        <v>79</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>96</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>97</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>97</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>101</v>
+        <v>79</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" t="s">
+        <v>79</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" t="s">
+        <v>78</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>52</v>
+      </c>
+      <c r="C57" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>53</v>
       </c>
-      <c r="C55" t="s">
-        <v>96</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>54</v>
-      </c>
-      <c r="B58" t="s">
-        <v>55</v>
-      </c>
       <c r="C58" t="s">
-        <v>98</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>101</v>
+        <v>79</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>97</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>101</v>
+        <v>78</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" t="s">
+        <v>79</v>
+      </c>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" t="s">
         <v>57</v>
       </c>
-      <c r="C60" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>58</v>
-      </c>
-      <c r="C61" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>59</v>
-      </c>
       <c r="C62" t="s">
-        <v>97</v>
+        <v>79</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>97</v>
-      </c>
-      <c r="D63" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="C64" t="s">
-        <v>96</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="C65" t="s">
-        <v>96</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="C66" t="s">
-        <v>97</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" t="s">
+        <v>80</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69" t="s">
+        <v>60</v>
+      </c>
+      <c r="C69" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>61</v>
+      </c>
+      <c r="C70" t="s">
+        <v>79</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>62</v>
+      </c>
+      <c r="C71" t="s">
+        <v>79</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73" t="s">
         <v>64</v>
       </c>
-      <c r="C67" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>65</v>
-      </c>
-      <c r="C68" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>66</v>
-      </c>
-      <c r="C69" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" t="s">
-        <v>68</v>
-      </c>
-      <c r="C71" t="s">
-        <v>97</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>69</v>
-      </c>
-      <c r="C72" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>23</v>
-      </c>
       <c r="C73" t="s">
-        <v>97</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C74" t="s">
-        <v>97</v>
+        <v>80</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="C75" t="s">
-        <v>97</v>
+        <v>79</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="C76" t="s">
-        <v>98</v>
+        <v>80</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>71</v>
+      </c>
+      <c r="C77" t="s">
+        <v>79</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>70</v>
-      </c>
       <c r="B78" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C78" t="s">
-        <v>96</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C79" t="s">
-        <v>97</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="C80" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>74</v>
       </c>
       <c r="C81" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>75</v>
       </c>
       <c r="C82" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>76</v>
-      </c>
-      <c r="C83" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>67</v>
+      </c>
       <c r="B84" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C84" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="C85" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>78</v>
-      </c>
-      <c r="B87" t="s">
-        <v>79</v>
-      </c>
-      <c r="C87" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>80</v>
-      </c>
-      <c r="C88" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>81</v>
-      </c>
-      <c r="C89" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>82</v>
-      </c>
-      <c r="C90" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>87</v>
-      </c>
-      <c r="C91" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>88</v>
-      </c>
-      <c r="C92" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>89</v>
-      </c>
-      <c r="C93" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>90</v>
-      </c>
-      <c r="C94" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>66</v>
-      </c>
-      <c r="C95" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>86</v>
-      </c>
-      <c r="C96" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>91</v>
-      </c>
-      <c r="C97" t="s">
-        <v>96</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>92</v>
-      </c>
-      <c r="C98" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>83</v>
-      </c>
-      <c r="B100" t="s">
-        <v>84</v>
-      </c>
-      <c r="C100" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>85</v>
-      </c>
-      <c r="C101" t="s">
-        <v>96</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>66</v>
-      </c>
-      <c r="C102" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>86</v>
-      </c>
-      <c r="C103" t="s">
-        <v>97</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>55</v>
+      </c>
+      <c r="C86" t="s">
+        <v>79</v>
+      </c>
+      <c r="D86" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
feat(doc): adicionar mais feitos ao documento de testes
</commit_message>
<xml_diff>
--- a/documentacao/teste_maisconsulta.xlsx
+++ b/documentacao/teste_maisconsulta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\--consulta\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2801B7D-FB16-4D72-B673-209431A8BFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D5C159-0B08-4D9F-800C-22A7A94CE12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F13FDC1B-4AD5-47E7-AA19-1D28F11FE616}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="84">
   <si>
     <t>Testes do sistema</t>
   </si>
@@ -250,9 +250,6 @@
   </si>
   <si>
     <t>Rever input checkable</t>
-  </si>
-  <si>
-    <t>Select está com estilização diferente</t>
   </si>
   <si>
     <t>Sinalizar campos obrigatórios</t>
@@ -658,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67F6240-8D79-49A4-8FA5-5E1579F8B412}">
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,10 +674,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -691,7 +688,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -700,7 +697,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -709,7 +706,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -718,7 +715,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -727,7 +724,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -736,7 +733,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -745,7 +742,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -760,7 +757,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -769,7 +766,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -778,7 +775,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -787,7 +784,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -796,7 +793,7 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -805,7 +802,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -814,7 +811,7 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -823,7 +820,7 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" s="2"/>
     </row>
@@ -832,7 +829,7 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D18" s="2"/>
     </row>
@@ -841,7 +838,7 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D19" s="2"/>
     </row>
@@ -850,7 +847,7 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -859,7 +856,7 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -868,7 +865,7 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D22" s="2"/>
     </row>
@@ -877,7 +874,7 @@
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D23" s="2"/>
     </row>
@@ -892,7 +889,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D25" s="2"/>
     </row>
@@ -901,7 +898,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" s="2"/>
     </row>
@@ -910,7 +907,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D27" s="2"/>
     </row>
@@ -928,7 +925,7 @@
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D30" s="2"/>
     </row>
@@ -937,21 +934,21 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -959,7 +956,7 @@
         <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D33" s="2"/>
     </row>
@@ -968,7 +965,7 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D34" s="2"/>
     </row>
@@ -983,10 +980,10 @@
         <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -994,10 +991,10 @@
         <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1005,10 +1002,10 @@
         <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1016,10 +1013,10 @@
         <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1027,10 +1024,10 @@
         <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1038,10 +1035,10 @@
         <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1049,10 +1046,10 @@
         <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1060,10 +1057,10 @@
         <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1071,10 +1068,10 @@
         <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1082,10 +1079,10 @@
         <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1093,10 +1090,10 @@
         <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1104,10 +1101,10 @@
         <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1124,10 +1121,10 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1135,10 +1132,10 @@
         <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1146,16 +1143,18 @@
         <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>81</v>
-      </c>
-      <c r="D52" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D53" s="2"/>
     </row>
@@ -1164,10 +1163,10 @@
         <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1175,10 +1174,10 @@
         <v>50</v>
       </c>
       <c r="C55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1186,10 +1185,10 @@
         <v>51</v>
       </c>
       <c r="C56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1197,10 +1196,10 @@
         <v>52</v>
       </c>
       <c r="C57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1208,10 +1207,10 @@
         <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1219,10 +1218,10 @@
         <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,7 +1229,7 @@
         <v>55</v>
       </c>
       <c r="C60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D60" s="2"/>
     </row>
@@ -1245,10 +1244,10 @@
         <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1256,7 +1255,7 @@
         <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D63" s="2"/>
     </row>
@@ -1265,7 +1264,7 @@
         <v>23</v>
       </c>
       <c r="C64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D64" s="2"/>
     </row>
@@ -1274,7 +1273,7 @@
         <v>24</v>
       </c>
       <c r="C65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D65" s="2"/>
     </row>
@@ -1283,19 +1282,19 @@
         <v>25</v>
       </c>
       <c r="C66" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C67" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1309,7 +1308,7 @@
         <v>60</v>
       </c>
       <c r="C69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D69" s="2"/>
     </row>
@@ -1318,10 +1317,10 @@
         <v>61</v>
       </c>
       <c r="C70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1329,10 +1328,10 @@
         <v>62</v>
       </c>
       <c r="C71" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,19 +1345,21 @@
         <v>64</v>
       </c>
       <c r="C73" t="s">
-        <v>79</v>
-      </c>
-      <c r="D73" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>65</v>
       </c>
       <c r="C74" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1366,10 +1367,10 @@
         <v>66</v>
       </c>
       <c r="C75" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1377,10 +1378,10 @@
         <v>70</v>
       </c>
       <c r="C76" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1388,10 +1389,10 @@
         <v>71</v>
       </c>
       <c r="C77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1399,13 +1400,15 @@
         <v>72</v>
       </c>
       <c r="C78" t="s">
-        <v>79</v>
-      </c>
-      <c r="D78" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="C79" t="s">
         <v>78</v>
@@ -1414,12 +1417,14 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C80" t="s">
-        <v>79</v>
-      </c>
-      <c r="D80" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
@@ -1428,53 +1433,42 @@
       <c r="C81" t="s">
         <v>78</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="D81" s="2"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>75</v>
-      </c>
-      <c r="C82" t="s">
-        <v>79</v>
-      </c>
       <c r="D82" s="2"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" t="s">
+        <v>68</v>
+      </c>
+      <c r="C83" t="s">
+        <v>77</v>
+      </c>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>67</v>
-      </c>
       <c r="B84" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C84" t="s">
-        <v>78</v>
-      </c>
-      <c r="D84" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C85" t="s">
         <v>78</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>55</v>
-      </c>
-      <c r="C86" t="s">
-        <v>79</v>
-      </c>
-      <c r="D86" s="2"/>
+      <c r="D85" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
feat(front): adicionar ultimas modificações no front
</commit_message>
<xml_diff>
--- a/documentacao/teste_maisconsulta.xlsx
+++ b/documentacao/teste_maisconsulta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\--consulta\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D5C159-0B08-4D9F-800C-22A7A94CE12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA82466-E7D5-4C45-8270-5C0B7B29017E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F13FDC1B-4AD5-47E7-AA19-1D28F11FE616}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="83">
   <si>
     <t>Testes do sistema</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Backend deverá retornar o statusCode correto de acordo com o que aconteceu</t>
-  </si>
-  <si>
-    <t>Tela Home (Paciente)</t>
   </si>
   <si>
     <t>Notificações sem click</t>
@@ -292,7 +289,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,8 +305,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,6 +323,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,12 +345,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67F6240-8D79-49A4-8FA5-5E1579F8B412}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,10 +685,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,7 +699,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -697,25 +708,29 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -724,37 +739,37 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>78</v>
@@ -763,61 +778,61 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
         <v>77</v>
@@ -826,88 +841,92 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>78</v>
-      </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="2"/>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D27" s="2"/>
     </row>
@@ -915,243 +934,262 @@
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="2"/>
+      <c r="A29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="2"/>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" t="s">
-        <v>78</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" t="s">
-        <v>78</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" t="s">
-        <v>77</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
         <v>77</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C47" t="s">
         <v>77</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D48" s="2"/>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="2"/>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>44</v>
-      </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C53" t="s">
         <v>77</v>
@@ -1159,316 +1197,241 @@
       <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>49</v>
-      </c>
-      <c r="C54" t="s">
-        <v>78</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
       <c r="B55" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C56" t="s">
         <v>77</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C57" t="s">
         <v>77</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="C58" t="s">
-        <v>78</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C59" t="s">
         <v>77</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C60" t="s">
         <v>78</v>
       </c>
-      <c r="D60" s="2"/>
+      <c r="D60" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C62" t="s">
-        <v>78</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C63" t="s">
-        <v>78</v>
-      </c>
-      <c r="D63" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="C64" t="s">
-        <v>78</v>
-      </c>
-      <c r="D64" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>24</v>
-      </c>
-      <c r="C65" t="s">
-        <v>78</v>
-      </c>
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>62</v>
+      </c>
       <c r="B66" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C66" t="s">
-        <v>78</v>
-      </c>
-      <c r="D66" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C67" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D68" s="2"/>
+      <c r="B68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>59</v>
-      </c>
       <c r="B69" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C69" t="s">
-        <v>77</v>
-      </c>
-      <c r="D69" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C71" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>54</v>
+      </c>
+      <c r="C72" t="s">
+        <v>77</v>
+      </c>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>63</v>
-      </c>
       <c r="B73" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C73" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C74" t="s">
-        <v>79</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>66</v>
       </c>
-      <c r="C75" t="s">
-        <v>78</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C76" t="s">
-        <v>79</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>82</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C77" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="C78" t="s">
         <v>77</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>55</v>
-      </c>
-      <c r="C79" t="s">
-        <v>78</v>
-      </c>
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>73</v>
-      </c>
-      <c r="C80" t="s">
-        <v>77</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>74</v>
-      </c>
-      <c r="C81" t="s">
-        <v>78</v>
-      </c>
-      <c r="D81" s="2"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D82" s="2"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>67</v>
-      </c>
-      <c r="B83" t="s">
-        <v>68</v>
-      </c>
-      <c r="C83" t="s">
-        <v>77</v>
-      </c>
-      <c r="D83" s="2"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>69</v>
-      </c>
-      <c r="C84" t="s">
-        <v>77</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>55</v>
-      </c>
-      <c r="C85" t="s">
-        <v>78</v>
-      </c>
-      <c r="D85" s="2"/>
+      <c r="D78" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>